<commit_message>
changed template be + redisgn bulk upload
</commit_message>
<xml_diff>
--- a/app/excelTemplates/template_jadwaljumatan.xlsx
+++ b/app/excelTemplates/template_jadwaljumatan.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26926"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMESTER 5\Pengembangan Web\mission3\bismillah fix banget\Broadcast\app\excelTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\polban\sem 5\web dev challenge\app\excelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801725E4-A666-477B-B996-B3C300505973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC12E2B4-8091-49FE-9F32-050256C0CF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9108" yWindow="3396" windowWidth="10944" windowHeight="8964" xr2:uid="{4A92A4DA-1AF0-45A9-8378-A9FBACE63D64}"/>
+    <workbookView xWindow="-21720" yWindow="1245" windowWidth="21840" windowHeight="13020" xr2:uid="{4A92A4DA-1AF0-45A9-8378-A9FBACE63D64}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="INFO KODE" sheetId="2" r:id="rId2"/>
+    <sheet name="INPUT DISINI" sheetId="1" r:id="rId1"/>
+    <sheet name="INFO KODE (JANGAN DIUBAH)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nama Masjid</t>
   </si>
@@ -40,14 +40,32 @@
     <t>Nama Mubaligh</t>
   </si>
   <si>
-    <t>Tanggal Jumatan</t>
+    <t>Masjid</t>
+  </si>
+  <si>
+    <t>Mubaligh</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tanggal Jumatan
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>contoh: 12/31/2023</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +78,19 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -105,10 +136,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
@@ -450,26 +490,50 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="23" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="39" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{D57450FE-7D17-487F-87AD-D4E782191C80}">
+      <formula1>44927</formula1>
+      <formula2>2958101</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{563B7A9F-A5B1-4A57-A6C8-252CEA5674B2}">
+          <x14:formula1>
+            <xm:f>'INFO KODE (JANGAN DIUBAH)'!$B$2:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{877B08B8-0B8F-4BC7-8B4B-A4E2E7101677}">
+          <x14:formula1>
+            <xm:f>'INFO KODE (JANGAN DIUBAH)'!$F$2:$F$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -478,28 +542,30 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="5" max="5" width="17.875" customWidth="1"/>
+    <col min="6" max="6" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="39" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>